<commit_message>
Kapitel a vocab highlighted
</commit_message>
<xml_diff>
--- a/B2 Kurs Roadmap.xlsx
+++ b/B2 Kurs Roadmap.xlsx
@@ -12,7 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="exam-B2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="41">
   <si>
     <t>Datum</t>
   </si>
@@ -99,6 +100,54 @@
   </si>
   <si>
     <t>Tag</t>
+  </si>
+  <si>
+    <t>Deutsch Grammatik wiederholung</t>
+  </si>
+  <si>
+    <t>(das ist wichtig fur mich-6, Adjektive Endungen und wiederholung)</t>
+  </si>
+  <si>
+    <t>Beziehung zu dinge( bis 6 part)</t>
+  </si>
+  <si>
+    <t>Kapitel 1</t>
+  </si>
+  <si>
+    <t>Kapitel 2</t>
+  </si>
+  <si>
+    <t>Kapitel 3</t>
+  </si>
+  <si>
+    <t>Kapitel 4</t>
+  </si>
+  <si>
+    <t>Kapitel 5</t>
+  </si>
+  <si>
+    <t>Kapitel 6</t>
+  </si>
+  <si>
+    <t>Kapitel 7</t>
+  </si>
+  <si>
+    <t>Kapitel 8</t>
+  </si>
+  <si>
+    <t>Kapitel 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Kapitel 10</t>
+  </si>
+  <si>
+    <t>Kapitel 11</t>
+  </si>
+  <si>
+    <t>Kapitel 12</t>
   </si>
 </sst>
 </file>
@@ -106,7 +155,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="[$-409]d\-mmm;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -184,7 +233,7 @@
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -193,7 +242,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -469,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F61"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,6 +565,591 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>45922</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>45923</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>45924</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>45925</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>45926</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>45927</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>45928</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>45929</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>45930</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>45931</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>45932</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>45933</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>45934</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>45935</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>45936</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>45937</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>45938</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>45939</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <v>45940</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
+        <v>45941</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+    </row>
+    <row r="22" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
+        <v>45942</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <v>45943</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+    </row>
+    <row r="24" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
+        <v>45944</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+    </row>
+    <row r="25" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
+        <v>45945</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+    </row>
+    <row r="26" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <v>45946</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+    </row>
+    <row r="27" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
+        <v>45947</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+    </row>
+    <row r="28" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
+        <v>45948</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+    </row>
+    <row r="29" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
+        <v>45949</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+    </row>
+    <row r="30" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
+        <v>45950</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+    </row>
+    <row r="31" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A31" s="2">
+        <v>45951</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+    </row>
+    <row r="32" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A32" s="2">
+        <v>45952</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+    </row>
+    <row r="33" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A33" s="2">
+        <v>45953</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+    </row>
+    <row r="34" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A34" s="2">
+        <v>45954</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+    </row>
+    <row r="35" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A35" s="2">
+        <v>45955</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" s="3"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+    </row>
+    <row r="36" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A36" s="2">
+        <v>45956</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+    </row>
+    <row r="37" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A37" s="2">
+        <v>45957</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" s="3"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+    </row>
+    <row r="38" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A38" s="2">
+        <v>45958</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" s="3"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+    </row>
+    <row r="39" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A39" s="2">
+        <v>45959</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39" s="3"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+    </row>
+    <row r="40" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A40" s="2">
+        <v>45960</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C40" s="3"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+    </row>
+    <row r="41" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A41" s="2">
+        <v>45961</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" s="3"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"sat"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F61"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="64.140625" customWidth="1"/>
+    <col min="5" max="5" width="59.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
     <row r="2" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>45902</v>
@@ -515,9 +1160,15 @@
       <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
+      <c r="D2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2">

</xml_diff>

<commit_message>
kapitel 1 update- incomplete
</commit_message>
<xml_diff>
--- a/B2 Kurs Roadmap.xlsx
+++ b/B2 Kurs Roadmap.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\German lanugage\Deutsch-B2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\German lanugage\B2 Kurs Material Update\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CDDEA41-3C08-4415-8796-682505111D21}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7752" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="exam-B2" sheetId="2" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="44">
   <si>
     <t>Datum</t>
   </si>
@@ -148,12 +149,21 @@
   </si>
   <si>
     <t>Kapitel 12</t>
+  </si>
+  <si>
+    <t>problem mit adjektivendung (ohne artikel)</t>
+  </si>
+  <si>
+    <t>ja</t>
+  </si>
+  <si>
+    <t>Beziehung zu Dinge(nicht: Familie,Freundschaft)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
@@ -528,24 +538,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="64.140625" customWidth="1"/>
-    <col min="5" max="5" width="59.7109375" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="64.109375" customWidth="1"/>
+    <col min="5" max="5" width="59.6640625" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -565,7 +575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>45922</v>
       </c>
@@ -579,7 +589,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>45923</v>
       </c>
@@ -589,11 +599,17 @@
       <c r="C3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>45924</v>
       </c>
@@ -607,7 +623,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>45925</v>
       </c>
@@ -621,7 +637,7 @@
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>45926</v>
       </c>
@@ -635,7 +651,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>45927</v>
       </c>
@@ -649,7 +665,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>45928</v>
       </c>
@@ -663,7 +679,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>45929</v>
       </c>
@@ -677,7 +693,7 @@
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>45930</v>
       </c>
@@ -691,7 +707,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>45931</v>
       </c>
@@ -705,7 +721,7 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>45932</v>
       </c>
@@ -719,7 +735,7 @@
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>45933</v>
       </c>
@@ -733,7 +749,7 @@
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>45934</v>
       </c>
@@ -747,7 +763,7 @@
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>45935</v>
       </c>
@@ -761,7 +777,7 @@
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>45936</v>
       </c>
@@ -775,7 +791,7 @@
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>45937</v>
       </c>
@@ -789,7 +805,7 @@
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>45938</v>
       </c>
@@ -803,7 +819,7 @@
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>45939</v>
       </c>
@@ -817,7 +833,7 @@
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>45940</v>
       </c>
@@ -831,7 +847,7 @@
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>45941</v>
       </c>
@@ -845,7 +861,7 @@
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>45942</v>
       </c>
@@ -859,7 +875,7 @@
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>45943</v>
       </c>
@@ -873,7 +889,7 @@
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>45944</v>
       </c>
@@ -887,7 +903,7 @@
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>45945</v>
       </c>
@@ -901,7 +917,7 @@
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>45946</v>
       </c>
@@ -915,7 +931,7 @@
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>45947</v>
       </c>
@@ -929,7 +945,7 @@
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>45948</v>
       </c>
@@ -943,7 +959,7 @@
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>45949</v>
       </c>
@@ -957,7 +973,7 @@
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>45950</v>
       </c>
@@ -969,7 +985,7 @@
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>45951</v>
       </c>
@@ -981,7 +997,7 @@
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>45952</v>
       </c>
@@ -993,7 +1009,7 @@
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
     </row>
-    <row r="33" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>45953</v>
       </c>
@@ -1005,7 +1021,7 @@
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
     </row>
-    <row r="34" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
         <v>45954</v>
       </c>
@@ -1017,7 +1033,7 @@
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
     </row>
-    <row r="35" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
         <v>45955</v>
       </c>
@@ -1029,7 +1045,7 @@
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
     </row>
-    <row r="36" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
         <v>45956</v>
       </c>
@@ -1041,7 +1057,7 @@
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
     </row>
-    <row r="37" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>45957</v>
       </c>
@@ -1053,7 +1069,7 @@
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
     </row>
-    <row r="38" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
         <v>45958</v>
       </c>
@@ -1065,7 +1081,7 @@
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
     </row>
-    <row r="39" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
         <v>45959</v>
       </c>
@@ -1077,7 +1093,7 @@
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
     </row>
-    <row r="40" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
         <v>45960</v>
       </c>
@@ -1089,7 +1105,7 @@
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
     </row>
-    <row r="41" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
         <v>45961</v>
       </c>
@@ -1113,24 +1129,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="64.140625" customWidth="1"/>
-    <col min="5" max="5" width="59.7109375" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="64.109375" customWidth="1"/>
+    <col min="5" max="5" width="59.6640625" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1150,7 +1166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>45902</v>
       </c>
@@ -1170,7 +1186,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>45903</v>
       </c>
@@ -1184,7 +1200,7 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>45904</v>
       </c>
@@ -1198,7 +1214,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>45905</v>
       </c>
@@ -1212,7 +1228,7 @@
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>45906</v>
       </c>
@@ -1224,7 +1240,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>45907</v>
       </c>
@@ -1238,7 +1254,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>45908</v>
       </c>
@@ -1252,7 +1268,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>45909</v>
       </c>
@@ -1266,7 +1282,7 @@
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>45910</v>
       </c>
@@ -1280,7 +1296,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>45911</v>
       </c>
@@ -1294,7 +1310,7 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>45912</v>
       </c>
@@ -1308,7 +1324,7 @@
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>45913</v>
       </c>
@@ -1320,7 +1336,7 @@
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>45914</v>
       </c>
@@ -1334,7 +1350,7 @@
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>45915</v>
       </c>
@@ -1348,7 +1364,7 @@
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>45916</v>
       </c>
@@ -1362,7 +1378,7 @@
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>45917</v>
       </c>
@@ -1376,7 +1392,7 @@
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>45918</v>
       </c>
@@ -1390,7 +1406,7 @@
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>45919</v>
       </c>
@@ -1404,7 +1420,7 @@
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>45920</v>
       </c>
@@ -1416,7 +1432,7 @@
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>45921</v>
       </c>
@@ -1430,7 +1446,7 @@
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>45922</v>
       </c>
@@ -1444,7 +1460,7 @@
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>45923</v>
       </c>
@@ -1458,7 +1474,7 @@
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>45924</v>
       </c>
@@ -1472,7 +1488,7 @@
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>45925</v>
       </c>
@@ -1486,7 +1502,7 @@
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>45926</v>
       </c>
@@ -1500,7 +1516,7 @@
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>45927</v>
       </c>
@@ -1512,7 +1528,7 @@
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>45928</v>
       </c>
@@ -1526,7 +1542,7 @@
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>45929</v>
       </c>
@@ -1540,7 +1556,7 @@
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>45930</v>
       </c>
@@ -1554,7 +1570,7 @@
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>45931</v>
       </c>
@@ -1568,7 +1584,7 @@
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>45932</v>
       </c>
@@ -1582,7 +1598,7 @@
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
     </row>
-    <row r="33" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>45933</v>
       </c>
@@ -1596,7 +1612,7 @@
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
     </row>
-    <row r="34" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
         <v>45934</v>
       </c>
@@ -1608,7 +1624,7 @@
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
     </row>
-    <row r="35" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
         <v>45935</v>
       </c>
@@ -1622,7 +1638,7 @@
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
     </row>
-    <row r="36" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
         <v>45936</v>
       </c>
@@ -1636,7 +1652,7 @@
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
     </row>
-    <row r="37" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>45937</v>
       </c>
@@ -1650,7 +1666,7 @@
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
     </row>
-    <row r="38" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
         <v>45938</v>
       </c>
@@ -1664,7 +1680,7 @@
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
     </row>
-    <row r="39" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
         <v>45939</v>
       </c>
@@ -1678,7 +1694,7 @@
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
     </row>
-    <row r="40" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
         <v>45940</v>
       </c>
@@ -1692,7 +1708,7 @@
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
     </row>
-    <row r="41" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
         <v>45941</v>
       </c>
@@ -1704,7 +1720,7 @@
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
     </row>
-    <row r="42" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
         <v>45942</v>
       </c>
@@ -1718,7 +1734,7 @@
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
     </row>
-    <row r="43" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
         <v>45943</v>
       </c>
@@ -1732,7 +1748,7 @@
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
     </row>
-    <row r="44" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A44" s="2">
         <v>45944</v>
       </c>
@@ -1746,7 +1762,7 @@
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
     </row>
-    <row r="45" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A45" s="2">
         <v>45945</v>
       </c>
@@ -1760,7 +1776,7 @@
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
     </row>
-    <row r="46" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A46" s="2">
         <v>45946</v>
       </c>
@@ -1774,7 +1790,7 @@
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
     </row>
-    <row r="47" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A47" s="2">
         <v>45947</v>
       </c>
@@ -1788,7 +1804,7 @@
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
     </row>
-    <row r="48" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A48" s="2">
         <v>45948</v>
       </c>
@@ -1800,7 +1816,7 @@
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
     </row>
-    <row r="49" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A49" s="2">
         <v>45949</v>
       </c>
@@ -1814,7 +1830,7 @@
       <c r="E49" s="4"/>
       <c r="F49" s="4"/>
     </row>
-    <row r="50" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A50" s="2">
         <v>45950</v>
       </c>
@@ -1828,7 +1844,7 @@
       <c r="E50" s="4"/>
       <c r="F50" s="4"/>
     </row>
-    <row r="51" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A51" s="2">
         <v>45951</v>
       </c>
@@ -1842,7 +1858,7 @@
       <c r="E51" s="4"/>
       <c r="F51" s="4"/>
     </row>
-    <row r="52" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A52" s="2">
         <v>45952</v>
       </c>
@@ -1856,7 +1872,7 @@
       <c r="E52" s="4"/>
       <c r="F52" s="4"/>
     </row>
-    <row r="53" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A53" s="2">
         <v>45953</v>
       </c>
@@ -1870,7 +1886,7 @@
       <c r="E53" s="4"/>
       <c r="F53" s="4"/>
     </row>
-    <row r="54" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A54" s="2">
         <v>45954</v>
       </c>
@@ -1884,7 +1900,7 @@
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
     </row>
-    <row r="55" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A55" s="2">
         <v>45955</v>
       </c>
@@ -1896,7 +1912,7 @@
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
     </row>
-    <row r="56" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A56" s="2">
         <v>45956</v>
       </c>
@@ -1910,7 +1926,7 @@
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
     </row>
-    <row r="57" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A57" s="2">
         <v>45957</v>
       </c>
@@ -1922,7 +1938,7 @@
       <c r="E57" s="4"/>
       <c r="F57" s="4"/>
     </row>
-    <row r="58" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A58" s="2">
         <v>45958</v>
       </c>
@@ -1934,7 +1950,7 @@
       <c r="E58" s="4"/>
       <c r="F58" s="4"/>
     </row>
-    <row r="59" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A59" s="2">
         <v>45959</v>
       </c>
@@ -1946,7 +1962,7 @@
       <c r="E59" s="4"/>
       <c r="F59" s="4"/>
     </row>
-    <row r="60" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A60" s="2">
         <v>45960</v>
       </c>
@@ -1958,7 +1974,7 @@
       <c r="E60" s="4"/>
       <c r="F60" s="4"/>
     </row>
-    <row r="61" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A61" s="2">
         <v>45961</v>
       </c>

</xml_diff>